<commit_message>
2nd half ready for orchestrator
</commit_message>
<xml_diff>
--- a/FirstHalf/ProiectRPA/PasswordManager.xlsx
+++ b/FirstHalf/ProiectRPA/PasswordManager.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laur\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laur\Desktop\RPA\proiect\RPA-PasswordManager\SecondHalf\SecondHalf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A69FBBBF-F631-4970-B6B6-BF3977F20918}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1979C4A2-5E60-4EDB-9372-7D0CE1B6DC24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10320" yWindow="5385" windowWidth="20910" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28035" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="46">
   <si>
     <t>Site-Name</t>
   </si>
@@ -43,43 +43,121 @@
     <t>https://www.google.com/intl/ro/gmail/about/#inbox</t>
   </si>
   <si>
+    <t>laurrpa@gmail.com</t>
+  </si>
+  <si>
+    <t>Laur-rpa1</t>
+  </si>
+  <si>
+    <t>PQy$G+UGf6?!gkeX</t>
+  </si>
+  <si>
+    <t>f3+^8@N9&amp;aXyMX@7</t>
+  </si>
+  <si>
     <t>https://auth.emag.ro/user/login</t>
   </si>
   <si>
-    <t>https://outlook.live.com/owa/0/?state=1&amp;redirectTo=aHR0cHM6Ly9vdXRsb29rLmxpdmUuY29tL21haWwvMC8</t>
+    <t>!4NcPTFhz2YqPpf7</t>
+  </si>
+  <si>
+    <t>Nh+ZT3ade+p^cM7W</t>
   </si>
   <si>
     <t>https://login.yahoo.com/?.lang=ro-RO&amp;.intl=ro&amp;src=homepage&amp;.done=https%3A%2F%2Fro.yahoo.com%2F%3Fp%3Dus&amp;pspid=2143930004&amp;activity=ybar-signin</t>
   </si>
   <si>
+    <t>dmg_00000@yahoo.com</t>
+  </si>
+  <si>
+    <t>Reddragon11</t>
+  </si>
+  <si>
+    <t>B5z7^%AP6Ve7VKp+</t>
+  </si>
+  <si>
+    <t>eYN6wdS^fk&amp;&amp;L7AP</t>
+  </si>
+  <si>
     <t>https://www.facebook.com/privacy/consent/user_cookie_choice/?source=pft_user_cookie_choice</t>
   </si>
   <si>
+    <t>LY+7rF5jcatS-=#J</t>
+  </si>
+  <si>
+    <t>*SZ9kbsuH7Y?!!eu</t>
+  </si>
+  <si>
     <t>https://www.linkedin.com/</t>
   </si>
   <si>
-    <t>Gmail</t>
-  </si>
-  <si>
-    <t>Emag</t>
-  </si>
-  <si>
-    <t>Outlook</t>
+    <t>s?9=y63%8wBwcLnv</t>
+  </si>
+  <si>
+    <t>&amp;&amp;#X3fAFnp=uae5U</t>
+  </si>
+  <si>
+    <t>https://discord.com/</t>
+  </si>
+  <si>
+    <t>sYL@d%q7+@ujnc62</t>
+  </si>
+  <si>
+    <t>*txAjsfKf_QT4k4E</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/</t>
+  </si>
+  <si>
+    <t>AC9a27XW?_%Z9LK^</t>
+  </si>
+  <si>
+    <t>GYHPe-pQgy#n8D4k</t>
+  </si>
+  <si>
+    <t>https://github.com/</t>
+  </si>
+  <si>
+    <t>2!@4fX+FjyEQA^r*</t>
+  </si>
+  <si>
+    <t>59$gsRq@gsPSQ9Zc</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/</t>
+  </si>
+  <si>
+    <t>xJ*=*93GnZr36TvG</t>
+  </si>
+  <si>
+    <t>rvV@WAfB39rfvLVZ</t>
+  </si>
+  <si>
+    <t>Google</t>
+  </si>
+  <si>
+    <t>Facebook</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>Reddit</t>
   </si>
   <si>
     <t>Yahoo</t>
   </si>
   <si>
-    <t>Facebook</t>
-  </si>
-  <si>
-    <t>Linkedin</t>
-  </si>
-  <si>
-    <t>laurrpa@gmail.com</t>
-  </si>
-  <si>
-    <t>Laur-rpa1</t>
+    <t>LinkedIn</t>
+  </si>
+  <si>
+    <t>Discord</t>
+  </si>
+  <si>
+    <t>Github</t>
+  </si>
+  <si>
+    <t>eMAG</t>
   </si>
 </sst>
 </file>
@@ -132,7 +210,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -143,7 +221,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -420,22 +497,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="23.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="255" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="27.42578125" customWidth="1"/>
     <col min="2" max="2" width="24.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="21.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="28.42578125" customWidth="1"/>
     <col min="5" max="5" width="21.5703125" customWidth="1"/>
+    <col min="6" max="6" width="70.140625" customWidth="1"/>
+    <col min="7" max="7" width="40.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -455,101 +534,244 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="45">
+    <row r="2" spans="1:7" ht="45" customHeight="1">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="30" customHeight="1">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="105" customHeight="1">
+      <c r="A4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" t="s">
         <v>18</v>
       </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="5" spans="1:7" ht="60" customHeight="1">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="30">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="75">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="D5" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="105">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="60">
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="30" customHeight="1">
       <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>18</v>
+        <v>42</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="30">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>18</v>
+        <v>25</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="B8" s="2"/>
-      <c r="C8" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="E7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="30" customHeight="1">
+      <c r="A8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="B11" s="2"/>
+      <c r="C11" s="3"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="B12"/>
+    </row>
+    <row r="16" spans="1:7" ht="75" customHeight="1">
+      <c r="B16" s="2"/>
+      <c r="C16"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" location="inbox" tooltip="https://www.google.com/intl/ro/gmail/about/#inbox" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="B3" r:id="rId2" tooltip="https://auth.emag.ro/user/login" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B7" r:id="rId6" tooltip="https://www.linkedin.com/" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="C2" r:id="rId7" xr:uid="{5818C394-B00C-44D4-8BCF-3335D06FFD6D}"/>
-    <hyperlink ref="C4" r:id="rId8" xr:uid="{2CF2A059-8B50-4F55-A1E3-627AC5F1D7D8}"/>
-    <hyperlink ref="C5" r:id="rId9" xr:uid="{5B860005-174B-41B8-891D-575233D3F2B0}"/>
-    <hyperlink ref="C6" r:id="rId10" xr:uid="{2BDA1F41-0323-4CA1-800F-A4C5A2C66FF2}"/>
-    <hyperlink ref="C7" r:id="rId11" xr:uid="{D0BEE573-B6DA-48ED-A049-B12129557EDE}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B6" r:id="rId4" tooltip="https://www.linkedin.com/" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C2" r:id="rId5" tooltip="mailto:laurrpa@gmail.com" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="C3" r:id="rId6" tooltip="mailto:laurrpa@gmail.com" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="C5" r:id="rId7" tooltip="mailto:laurrpa@gmail.com" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="C6" r:id="rId8" tooltip="mailto:laurrpa@gmail.com" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B7" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B8" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B9" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="C7" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="C8" r:id="rId13" tooltip="mailto:laurrpa@gmail.com" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="C9" r:id="rId14" tooltip="mailto:laurrpa@gmail.com" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B10" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="C10" r:id="rId16" tooltip="mailto:laurrpa@gmail.com" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="B4" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="C4" r:id="rId18" tooltip="mailto:dmg_00000@yahoo.com" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>